<commit_message>
Upgrade Lightstreamer client version to 6.0 and net7.0
</commit_message>
<xml_diff>
--- a/ExcelDemo_New.xlsx
+++ b/ExcelDemo_New.xlsx
@@ -62,10 +62,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
-    <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -129,12 +128,24 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5EB91E"/>
+        <bgColor rgb="FF339966"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF9C0006"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -176,8 +187,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+  <cellStyleXfs count="22">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -200,24 +211,14 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -230,92 +231,106 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Negative" xfId="20"/>
+    <cellStyle name="Positive" xfId="21"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -396,6 +411,20 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5EB91E"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <colors>
     <indexedColors>
@@ -441,7 +470,7 @@
       <rgbColor rgb="FFFFC7CE"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF5EB91E"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -465,15 +494,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>30960</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>69840</xdr:rowOff>
+      <xdr:colOff>122760</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>173520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2570760</xdr:colOff>
+      <xdr:colOff>2659680</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>30240</xdr:rowOff>
+      <xdr:rowOff>1440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -486,8 +515,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="30960" y="595440"/>
-          <a:ext cx="2539800" cy="532080"/>
+          <a:off x="122760" y="523800"/>
+          <a:ext cx="2536920" cy="529200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -530,13 +559,13 @@
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T26" activeCellId="0" sqref="T26"/>
+      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.12"/>
@@ -552,7 +581,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="e">
-        <f aca="false">rtd("lightstreamer.rtdnew23",,"CONFIG","https://push.lightstreamer.com/","","DEMO","QUOTE_ADAPTER","user_test","o93ujDNJasf,ajfih393!_ard3sfaklj_sjsijhdf3934eifaskik(2332334yh32rdusjdsshkahkhgfasif24egfwebkjbcfasik")</f>
+        <f aca="false">rtd("lightstreamer.rtdnew23",,"CONFIG","https://push.lightstreamer.com",,"WELCOME","STOCKS","user_test","o93ujDNJasf,ajfih393!_ard3sfaklj_sjsijhdf3934eifaskik(2332334yh32rdusjdsshkahkhgfasif24egfwebkjbcfasik")</f>
         <v>#NAME?</v>
       </c>
       <c r="B1" s="4"/>
@@ -572,7 +601,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="e">
-        <f aca="false">rtd("lightstreamer.rtdnew23",,"OPTIONS","max_frequency","0.2")</f>
+        <f aca="false">rtd("lightstreamer.rtdnew23",,"OPTIONS","max_frequency","1")</f>
         <v>#NAME?</v>
       </c>
       <c r="B2" s="4"/>
@@ -592,7 +621,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="e">
-        <f aca="false">rtd("lightstreamer.rtdnew23",,"OPTIONS","forced_transport","HTTP")</f>
+        <f aca="false">rtd("lightstreamer.rtdnew23",,"OPTIONS","forced_transport","WS")</f>
         <v>#NAME?</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -634,7 +663,7 @@
       <c r="N3" s="10"/>
       <c r="O3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4"/>
       <c r="B4" s="11" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item30","stock_name")</f>
@@ -687,7 +716,7 @@
       <c r="N4" s="15"/>
       <c r="O4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4"/>
       <c r="B5" s="16" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item29","stock_name")</f>
@@ -701,7 +730,7 @@
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item29","time")</f>
         <v>#NAME?</v>
       </c>
-      <c r="E5" s="19" t="e">
+      <c r="E5" s="14" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item29","pct_change")</f>
         <v>#NAME?</v>
       </c>
@@ -737,10 +766,10 @@
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item29","open_price")</f>
         <v>#NAME?</v>
       </c>
-      <c r="N5" s="20"/>
+      <c r="N5" s="19"/>
       <c r="O5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4"/>
       <c r="B6" s="11" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item28","stock_name")</f>
@@ -793,8 +822,11 @@
       <c r="N6" s="15"/>
       <c r="O6" s="4"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4"/>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="e">
+        <f aca="false">rtd("lightstreamer.rtdnew23",,"OPTIONS","stalled_timeout","7500")</f>
+        <v>#NAME?</v>
+      </c>
       <c r="B7" s="16" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item27","stock_name")</f>
         <v>#NAME?</v>
@@ -807,7 +839,7 @@
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item27","time")</f>
         <v>#NAME?</v>
       </c>
-      <c r="E7" s="19" t="e">
+      <c r="E7" s="14" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item27","pct_change")</f>
         <v>#NAME?</v>
       </c>
@@ -843,10 +875,10 @@
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item27","open_price")</f>
         <v>#NAME?</v>
       </c>
-      <c r="N7" s="20"/>
+      <c r="N7" s="19"/>
       <c r="O7" s="4"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4"/>
       <c r="B8" s="11" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item26","stock_name")</f>
@@ -899,7 +931,7 @@
       <c r="N8" s="15"/>
       <c r="O8" s="4"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4"/>
       <c r="B9" s="16" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item25","stock_name")</f>
@@ -913,7 +945,7 @@
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item25","time")</f>
         <v>#NAME?</v>
       </c>
-      <c r="E9" s="19" t="e">
+      <c r="E9" s="14" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item25","pct_change")</f>
         <v>#NAME?</v>
       </c>
@@ -949,10 +981,10 @@
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item25","open_price")</f>
         <v>#NAME?</v>
       </c>
-      <c r="N9" s="20"/>
+      <c r="N9" s="19"/>
       <c r="O9" s="4"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4"/>
       <c r="B10" s="11" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item24","stock_name")</f>
@@ -1005,7 +1037,7 @@
       <c r="N10" s="15"/>
       <c r="O10" s="4"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4"/>
       <c r="B11" s="16" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item23","stock_name")</f>
@@ -1019,7 +1051,7 @@
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item23","time")</f>
         <v>#NAME?</v>
       </c>
-      <c r="E11" s="19" t="e">
+      <c r="E11" s="14" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item23","pct_change")</f>
         <v>#NAME?</v>
       </c>
@@ -1055,10 +1087,10 @@
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item23","open_price")</f>
         <v>#NAME?</v>
       </c>
-      <c r="N11" s="20"/>
+      <c r="N11" s="19"/>
       <c r="O11" s="4"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4"/>
       <c r="B12" s="11" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item22","stock_name")</f>
@@ -1111,7 +1143,7 @@
       <c r="N12" s="15"/>
       <c r="O12" s="4"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4"/>
       <c r="B13" s="16" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item21","stock_name")</f>
@@ -1125,7 +1157,7 @@
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item21","time")</f>
         <v>#NAME?</v>
       </c>
-      <c r="E13" s="19" t="e">
+      <c r="E13" s="14" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item21","pct_change")</f>
         <v>#NAME?</v>
       </c>
@@ -1161,10 +1193,10 @@
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item21","open_price")</f>
         <v>#NAME?</v>
       </c>
-      <c r="N13" s="20"/>
+      <c r="N13" s="19"/>
       <c r="O13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4"/>
       <c r="B14" s="11" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item20","stock_name")</f>
@@ -1217,7 +1249,7 @@
       <c r="N14" s="15"/>
       <c r="O14" s="4"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4"/>
       <c r="B15" s="16" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item19","stock_name")</f>
@@ -1231,7 +1263,7 @@
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item19","time")</f>
         <v>#NAME?</v>
       </c>
-      <c r="E15" s="19" t="e">
+      <c r="E15" s="14" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item19","pct_change")</f>
         <v>#NAME?</v>
       </c>
@@ -1267,10 +1299,10 @@
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item19","open_price")</f>
         <v>#NAME?</v>
       </c>
-      <c r="N15" s="20"/>
+      <c r="N15" s="19"/>
       <c r="O15" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4"/>
       <c r="B16" s="11" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item18","stock_name")</f>
@@ -1323,7 +1355,7 @@
       <c r="N16" s="15"/>
       <c r="O16" s="4"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4"/>
       <c r="B17" s="16" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item17","stock_name")</f>
@@ -1337,7 +1369,7 @@
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item17","time")</f>
         <v>#NAME?</v>
       </c>
-      <c r="E17" s="19" t="e">
+      <c r="E17" s="14" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item17","pct_change")</f>
         <v>#NAME?</v>
       </c>
@@ -1373,10 +1405,10 @@
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item17","open_price")</f>
         <v>#NAME?</v>
       </c>
-      <c r="N17" s="20"/>
+      <c r="N17" s="19"/>
       <c r="O17" s="4"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4"/>
       <c r="B18" s="11" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item16","stock_name")</f>
@@ -1429,7 +1461,7 @@
       <c r="N18" s="15"/>
       <c r="O18" s="4"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4"/>
       <c r="B19" s="16" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item15","stock_name")</f>
@@ -1443,7 +1475,7 @@
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item15","time")</f>
         <v>#NAME?</v>
       </c>
-      <c r="E19" s="19" t="e">
+      <c r="E19" s="14" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item15","pct_change")</f>
         <v>#NAME?</v>
       </c>
@@ -1479,10 +1511,10 @@
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item15","open_price")</f>
         <v>#NAME?</v>
       </c>
-      <c r="N19" s="20"/>
+      <c r="N19" s="19"/>
       <c r="O19" s="4"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4"/>
       <c r="B20" s="11" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item14","stock_name")</f>
@@ -1535,7 +1567,7 @@
       <c r="N20" s="15"/>
       <c r="O20" s="4"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4"/>
       <c r="B21" s="16" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item13","stock_name")</f>
@@ -1549,7 +1581,7 @@
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item13","time")</f>
         <v>#NAME?</v>
       </c>
-      <c r="E21" s="19" t="e">
+      <c r="E21" s="14" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item13","pct_change")</f>
         <v>#NAME?</v>
       </c>
@@ -1585,10 +1617,10 @@
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item13","open_price")</f>
         <v>#NAME?</v>
       </c>
-      <c r="N21" s="20"/>
+      <c r="N21" s="19"/>
       <c r="O21" s="4"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4"/>
       <c r="B22" s="11" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item12","stock_name")</f>
@@ -1641,7 +1673,7 @@
       <c r="N22" s="15"/>
       <c r="O22" s="4"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4"/>
       <c r="B23" s="16" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item11","stock_name")</f>
@@ -1655,7 +1687,7 @@
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item11","time")</f>
         <v>#NAME?</v>
       </c>
-      <c r="E23" s="19" t="e">
+      <c r="E23" s="14" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item11","pct_change")</f>
         <v>#NAME?</v>
       </c>
@@ -1691,10 +1723,10 @@
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item11","open_price")</f>
         <v>#NAME?</v>
       </c>
-      <c r="N23" s="20"/>
+      <c r="N23" s="19"/>
       <c r="O23" s="4"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4"/>
       <c r="B24" s="11" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item10","stock_name")</f>
@@ -1747,7 +1779,7 @@
       <c r="N24" s="15"/>
       <c r="O24" s="4"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4"/>
       <c r="B25" s="16" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item9","stock_name")</f>
@@ -1761,7 +1793,7 @@
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item9","time")</f>
         <v>#NAME?</v>
       </c>
-      <c r="E25" s="19" t="e">
+      <c r="E25" s="14" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item9","pct_change")</f>
         <v>#NAME?</v>
       </c>
@@ -1797,10 +1829,10 @@
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item9","open_price")</f>
         <v>#NAME?</v>
       </c>
-      <c r="N25" s="20"/>
+      <c r="N25" s="19"/>
       <c r="O25" s="4"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4"/>
       <c r="B26" s="11" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item8","stock_name")</f>
@@ -1853,7 +1885,7 @@
       <c r="N26" s="15"/>
       <c r="O26" s="4"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4"/>
       <c r="B27" s="16" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item7","stock_name")</f>
@@ -1867,7 +1899,7 @@
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item7","time")</f>
         <v>#NAME?</v>
       </c>
-      <c r="E27" s="19" t="e">
+      <c r="E27" s="14" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item7","pct_change")</f>
         <v>#NAME?</v>
       </c>
@@ -1903,10 +1935,10 @@
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item7","open_price")</f>
         <v>#NAME?</v>
       </c>
-      <c r="N27" s="20"/>
+      <c r="N27" s="19"/>
       <c r="O27" s="4"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4"/>
       <c r="B28" s="11" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item6","stock_name")</f>
@@ -1959,7 +1991,7 @@
       <c r="N28" s="15"/>
       <c r="O28" s="4"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4"/>
       <c r="B29" s="16" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item5","stock_name")</f>
@@ -1973,7 +2005,7 @@
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item5","time")</f>
         <v>#NAME?</v>
       </c>
-      <c r="E29" s="19" t="e">
+      <c r="E29" s="14" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item5","pct_change")</f>
         <v>#NAME?</v>
       </c>
@@ -2009,10 +2041,10 @@
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item5","open_price")</f>
         <v>#NAME?</v>
       </c>
-      <c r="N29" s="20"/>
+      <c r="N29" s="19"/>
       <c r="O29" s="4"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4"/>
       <c r="B30" s="11" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item4","stock_name")</f>
@@ -2065,7 +2097,7 @@
       <c r="N30" s="15"/>
       <c r="O30" s="4"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4"/>
       <c r="B31" s="16" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item3","stock_name")</f>
@@ -2079,7 +2111,7 @@
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item3","time")</f>
         <v>#NAME?</v>
       </c>
-      <c r="E31" s="19" t="e">
+      <c r="E31" s="14" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item3","pct_change")</f>
         <v>#NAME?</v>
       </c>
@@ -2115,10 +2147,10 @@
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item3","open_price")</f>
         <v>#NAME?</v>
       </c>
-      <c r="N31" s="20"/>
+      <c r="N31" s="19"/>
       <c r="O31" s="4"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4"/>
       <c r="B32" s="11" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item2","stock_name")</f>
@@ -2171,7 +2203,7 @@
       <c r="N32" s="15"/>
       <c r="O32" s="4"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4"/>
       <c r="B33" s="16" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item1","stock_name")</f>
@@ -2185,7 +2217,7 @@
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item1","time")</f>
         <v>#NAME?</v>
       </c>
-      <c r="E33" s="19" t="e">
+      <c r="E33" s="14" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item1","pct_change")</f>
         <v>#NAME?</v>
       </c>
@@ -2221,10 +2253,10 @@
         <f aca="false">rtd("lightstreamer.rtdnew23",,"item1","open_price")</f>
         <v>#NAME?</v>
       </c>
-      <c r="N33" s="20"/>
+      <c r="N33" s="19"/>
       <c r="O33" s="4"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="5"/>
@@ -2241,7 +2273,7 @@
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="5"/>
@@ -2258,8 +2290,8 @@
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="21" t="e">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="20" t="e">
         <f aca="false">rtd("lightstreamer.rtdnew23",,"LAST","")</f>
         <v>#NAME?</v>
       </c>
@@ -2279,84 +2311,87 @@
       <c r="O36" s="4"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="22"/>
-      <c r="B37" s="23"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="24"/>
-      <c r="I37" s="24"/>
-      <c r="J37" s="24"/>
-      <c r="K37" s="24"/>
-      <c r="L37" s="24"/>
-      <c r="M37" s="24"/>
-      <c r="N37" s="23"/>
+      <c r="A37" s="21" t="e">
+        <f aca="false">rtd("lightstreamer.rtdnew23",,"PX","")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B37" s="22"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="23"/>
+      <c r="J37" s="23"/>
+      <c r="K37" s="23"/>
+      <c r="L37" s="23"/>
+      <c r="M37" s="23"/>
+      <c r="N37" s="22"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="23"/>
-      <c r="B38" s="23"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="24"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="24"/>
-      <c r="I38" s="24"/>
-      <c r="J38" s="24"/>
-      <c r="K38" s="24"/>
-      <c r="L38" s="24"/>
-      <c r="M38" s="24"/>
-      <c r="N38" s="23"/>
+      <c r="A38" s="22"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="23"/>
+      <c r="J38" s="23"/>
+      <c r="K38" s="23"/>
+      <c r="L38" s="23"/>
+      <c r="M38" s="23"/>
+      <c r="N38" s="22"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="23"/>
-      <c r="B39" s="23"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="24"/>
-      <c r="I39" s="24"/>
-      <c r="J39" s="24"/>
-      <c r="K39" s="24"/>
-      <c r="L39" s="24"/>
-      <c r="M39" s="24"/>
-      <c r="N39" s="23"/>
+      <c r="A39" s="22"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="23"/>
+      <c r="J39" s="23"/>
+      <c r="K39" s="23"/>
+      <c r="L39" s="23"/>
+      <c r="M39" s="23"/>
+      <c r="N39" s="22"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="23"/>
-      <c r="B40" s="23"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="24"/>
-      <c r="H40" s="24"/>
-      <c r="I40" s="24"/>
-      <c r="J40" s="24"/>
-      <c r="K40" s="24"/>
-      <c r="L40" s="24"/>
-      <c r="M40" s="24"/>
-      <c r="N40" s="23"/>
+      <c r="A40" s="22"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="23"/>
+      <c r="H40" s="23"/>
+      <c r="I40" s="23"/>
+      <c r="J40" s="23"/>
+      <c r="K40" s="23"/>
+      <c r="L40" s="23"/>
+      <c r="M40" s="23"/>
+      <c r="N40" s="22"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="23"/>
-      <c r="B41" s="23"/>
-      <c r="C41" s="24"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="24"/>
-      <c r="F41" s="24"/>
-      <c r="G41" s="24"/>
-      <c r="H41" s="24"/>
-      <c r="I41" s="24"/>
-      <c r="J41" s="24"/>
-      <c r="K41" s="24"/>
-      <c r="L41" s="24"/>
-      <c r="M41" s="24"/>
-      <c r="N41" s="23"/>
+      <c r="A41" s="22"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="23"/>
+      <c r="H41" s="23"/>
+      <c r="I41" s="23"/>
+      <c r="J41" s="23"/>
+      <c r="K41" s="23"/>
+      <c r="L41" s="23"/>
+      <c r="M41" s="23"/>
+      <c r="N41" s="22"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1">
@@ -2387,8 +2422,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E33">
-    <cfRule type="containsText" priority="9" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="." dxfId="7">
-      <formula>NOT(ISERROR(SEARCH(".",E4)))</formula>
+    <cfRule type="notContainsText" priority="9" operator="notContains" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="-" dxfId="7">
+      <formula>ISERROR(SEARCH("-",E4))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:E33">
+    <cfRule type="containsText" priority="10" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="-" dxfId="1">
+      <formula>NOT(ISERROR(SEARCH("-",E4)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="11" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>